<commit_message>
T1: Repaired ex100 to 100c
</commit_message>
<xml_diff>
--- a/Fizyka_Sprawka/Lab2_Cw57c/Final_Sheet/Ex9,10.xlsx
+++ b/Fizyka_Sprawka/Lab2_Cw57c/Final_Sheet/Ex9,10.xlsx
@@ -26,9 +26,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
-    <t xml:space="preserve"> Nie mogłem znaleźć literatury w której byłaby tabela koncentracji swobodnych nośników ładunku</t>
-  </si>
-  <si>
     <t>10. Uzyskane wartości parametrów gammaB i n porównać z danymi literaturowymi oraz określić rodzaj materiału, z którego wykonany był badany hallotron.</t>
   </si>
   <si>
@@ -51,6 +48,9 @@
   </si>
   <si>
     <t>9. Obliczyć koncentrację n swobodnych nośników ładunku oraz jej niepewność.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Hallotron zosta wytworzony z półprzewodnika.</t>
   </si>
 </sst>
 </file>
@@ -8378,8 +8378,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G37" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8390,7 +8390,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1" s="22"/>
       <c r="C1" s="22"/>
@@ -8403,10 +8403,10 @@
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" s="25"/>
       <c r="D2" s="5"/>
@@ -8417,7 +8417,7 @@
     </row>
     <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="18"/>
       <c r="C3" s="17"/>
@@ -8429,11 +8429,11 @@
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="16"/>
       <c r="C4" s="15" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
@@ -8447,7 +8447,7 @@
         <v>353.2944756</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
@@ -8473,7 +8473,7 @@
         <v>34</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
@@ -8663,7 +8663,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="26" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B26" s="27"/>
       <c r="C26" s="27"/>
@@ -8683,9 +8683,9 @@
       <c r="G27" s="30"/>
       <c r="H27" s="31"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="26" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B28" s="27"/>
       <c r="C28" s="27"/>

</xml_diff>